<commit_message>
Bernard Updated Test Results Sheet
</commit_message>
<xml_diff>
--- a/Consumer Debt Kaggle - Algo-Results.xlsx
+++ b/Consumer Debt Kaggle - Algo-Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Manual</t>
   </si>
   <si>
-    <t>Wining Snapshot</t>
-  </si>
-  <si>
     <t>Bernard</t>
   </si>
   <si>
@@ -172,6 +169,12 @@
   </si>
   <si>
     <t>XGB Rnd 7641,3431,1270,8939,9101 /  boost exponential / adaboost</t>
+  </si>
+  <si>
+    <t>#50 - Top 5%</t>
+  </si>
+  <si>
+    <t>XGB Rnd 7641,3431,1270,8939,9101 /  boost deviance / adaboost</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,10 +1445,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>43</v>
@@ -1475,16 +1478,55 @@
         <v>0.86830099999999999</v>
       </c>
       <c r="L31" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="C32" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="7">
+        <v>10</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="18">
+        <v>5</v>
+      </c>
+      <c r="J32" s="10">
+        <v>0.86614999999999998</v>
+      </c>
+      <c r="K32" s="30">
+        <v>0.86812</v>
+      </c>
+      <c r="L32" s="30" t="s">
         <v>48</v>
       </c>
+      <c r="M32" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="21" t="s">
-        <v>44</v>
-      </c>
+      <c r="B35" s="21"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M37" s="3"/>

</xml_diff>

<commit_message>
Added Testing updates from Nanda
</commit_message>
<xml_diff>
--- a/Consumer Debt Kaggle - Algo-Results.xlsx
+++ b/Consumer Debt Kaggle - Algo-Results.xlsx
@@ -1,29 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trichna\Documents\NYCDSA\Capstone\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Single Algos" sheetId="1" r:id="rId1"/>
     <sheet name="Ensembles" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -185,15 +190,72 @@
   </si>
   <si>
     <t>#64</t>
+  </si>
+  <si>
+    <t>GBM - Manual
+XGB - Hyperopt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #39</t>
+  </si>
+  <si>
+    <t>GBM - max_features = log2, XGB - Best combination from Hyperopt</t>
+  </si>
+  <si>
+    <t>#59</t>
+  </si>
+  <si>
+    <t>GBM - max_features = auto, XGB - Best combination from Hyperopt</t>
+  </si>
+  <si>
+    <t>#44</t>
+  </si>
+  <si>
+    <t>GBM - max_features = 0.3, XGB - Best combination from Hyperopt</t>
+  </si>
+  <si>
+    <t>GBM - max_features = 0.2, XGB - Best combination from Hyperopt</t>
+  </si>
+  <si>
+    <t>GBM - max_features = 0.1, XGB - Best combination from Hyperopt</t>
+  </si>
+  <si>
+    <t>#45</t>
+  </si>
+  <si>
+    <t>GBM - max_features = 0.15, XGB - Best combination from Hyperopt</t>
+  </si>
+  <si>
+    <t>#42</t>
+  </si>
+  <si>
+    <t>GBM - n_estimators=197, max_depth=5,            min_samples_split=319,  min_samples_leaf=89, max_features='log2', XGB - Best combination from Hyperopt</t>
+  </si>
+  <si>
+    <t># 53</t>
+  </si>
+  <si>
+    <t>GBM - BayesOpt
+XGB - Hyperopt</t>
+  </si>
+  <si>
+    <t>GBM - n_estimators=197, max_depth=5,            min_samples_split=319,  min_samples_leaf=89, max_features='log2', random_state = 1234,XGB - Best combination from Hyperopt</t>
+  </si>
+  <si>
+    <t># 63</t>
+  </si>
+  <si>
+    <t>#33 - Top 3%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -293,7 +355,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -382,6 +444,24 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -657,7 +737,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -668,34 +748,34 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="9" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="9" customWidth="1"/>
-    <col min="11" max="12" width="13.6640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="9" customWidth="1"/>
+    <col min="11" max="12" width="13.7109375" style="10" customWidth="1"/>
     <col min="13" max="13" width="98" style="4" customWidth="1"/>
-    <col min="14" max="14" width="44.6640625" style="21" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="6"/>
+    <col min="14" max="14" width="44.7109375" style="21" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -736,7 +816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -749,7 +829,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="27"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>17</v>
       </c>
@@ -764,7 +844,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="27"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -777,7 +857,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="27"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -790,7 +870,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="27"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -803,7 +883,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="27"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>21</v>
       </c>
@@ -818,7 +898,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="27"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -831,7 +911,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="27"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
@@ -868,7 +948,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>9</v>
       </c>
@@ -904,7 +984,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
@@ -941,7 +1021,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
@@ -978,7 +1058,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>50</v>
       </c>
@@ -1019,7 +1099,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>9</v>
       </c>
@@ -1055,7 +1135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>9</v>
       </c>
@@ -1091,7 +1171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
@@ -1163,7 +1243,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>9</v>
       </c>
@@ -1199,7 +1279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>9</v>
       </c>
@@ -1235,22 +1315,22 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="M23" s="29"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>22</v>
       </c>
@@ -1260,7 +1340,7 @@
       <c r="J26" s="18"/>
       <c r="M26" s="23"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>9</v>
       </c>
@@ -1297,7 +1377,7 @@
       </c>
       <c r="N27" s="24"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>9</v>
       </c>
@@ -1333,7 +1413,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +1449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +1485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>9</v>
       </c>
@@ -1441,7 +1521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>9</v>
       </c>
@@ -1478,7 +1558,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>9</v>
       </c>
@@ -1519,7 +1599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>44</v>
       </c>
@@ -1560,7 +1640,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>44</v>
       </c>
@@ -1601,34 +1681,342 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
-      <c r="B38" s="21"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="M40" s="3"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="M42" s="3"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="M43" s="3"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="M44" s="3"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="M45" s="3"/>
-    </row>
-    <row r="46" spans="1:13">
+    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="32">
+        <v>10</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="35">
+        <v>5</v>
+      </c>
+      <c r="J38" s="36">
+        <v>0.86606000000000005</v>
+      </c>
+      <c r="K38" s="36">
+        <v>0.86841699999999999</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="32">
+        <v>10</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I39" s="35">
+        <v>5</v>
+      </c>
+      <c r="J39" s="36">
+        <v>0.86591300000000004</v>
+      </c>
+      <c r="K39" s="36">
+        <v>0.86795999999999995</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="32">
+        <v>10</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" s="35">
+        <v>5</v>
+      </c>
+      <c r="J40" s="36">
+        <v>0.86592000000000002</v>
+      </c>
+      <c r="K40" s="36">
+        <v>0.86827900000000002</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="32">
+        <v>10</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" s="35">
+        <v>5</v>
+      </c>
+      <c r="J41" s="36">
+        <v>0.86602599999999996</v>
+      </c>
+      <c r="K41" s="36">
+        <v>0.86849299999999996</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="32">
+        <v>10</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" s="35">
+        <v>5</v>
+      </c>
+      <c r="J42" s="36">
+        <v>0.865873</v>
+      </c>
+      <c r="K42" s="36">
+        <v>0.86824199999999996</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="32">
+        <v>10</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I43" s="35">
+        <v>5</v>
+      </c>
+      <c r="J43" s="36">
+        <v>0.86601399999999995</v>
+      </c>
+      <c r="K43" s="36">
+        <v>0.86833899999999997</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="32">
+        <v>10</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" s="35">
+        <v>5</v>
+      </c>
+      <c r="J44" s="36">
+        <v>0.86590999999999996</v>
+      </c>
+      <c r="K44" s="36">
+        <v>0.86807000000000001</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="32">
+        <v>10</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H45" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45" s="35">
+        <v>5</v>
+      </c>
+      <c r="J45" s="36">
+        <v>0.86594000000000004</v>
+      </c>
+      <c r="K45" s="36">
+        <v>0.86790500000000004</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="31"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M48" s="3"/>
     </row>
   </sheetData>
@@ -1650,14 +2038,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
results after testing FE
</commit_message>
<xml_diff>
--- a/Consumer Debt Kaggle - Algo-Results.xlsx
+++ b/Consumer Debt Kaggle - Algo-Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\nycdsa\Projects\05-Kaggle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trichna\Documents\NYCDSA\Capstone\data\FE\Git upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Algos Models" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="97">
   <si>
     <t>Algorithm</t>
   </si>
@@ -280,6 +280,53 @@
   </si>
   <si>
     <t>#53 - Top 6%</t>
+  </si>
+  <si>
+    <t>0.86533</t>
+  </si>
+  <si>
+    <t>#91</t>
+  </si>
+  <si>
+    <t>0.86541</t>
+  </si>
+  <si>
+    <t>#93</t>
+  </si>
+  <si>
+    <t>0.863254</t>
+  </si>
+  <si>
+    <t>GBM - max_features = 0.2, XGB - Best combination from Hyperopt
+Used cs-training-combine-f07 &amp; cs-test-combine-f07  files</t>
+  </si>
+  <si>
+    <t>GBM - max_features = 0.2, XGB - Best combination from Hyperopt
+Used training-outlier-weight-f08 &amp; test-outlier-weight-f08 files</t>
+  </si>
+  <si>
+    <t>GBM - max_features =log2, XGB - Best combination from Hyperopt
+Used training-outlier-weight-f08 &amp; test-outlier-weight-f08 files</t>
+  </si>
+  <si>
+    <t>#224</t>
+  </si>
+  <si>
+    <t>GBM - max_features = 0.2, XGB - Best combination from Hyperopt
+Used cs-training-outlier-agerisk-f10 &amp; cs-test-outlier-agerisk-f10  files</t>
+  </si>
+  <si>
+    <t>0.865137</t>
+  </si>
+  <si>
+    <t>0.86337</t>
+  </si>
+  <si>
+    <t>#242</t>
+  </si>
+  <si>
+    <t>GBM - max_features = 0.2, XGB - Best combination from Hyperopt
+Used cs-training-outlier-debt-f09 &amp; cs-test-outlier-debt-f09  files</t>
   </si>
 </sst>
 </file>
@@ -382,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -452,9 +499,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -781,11 +825,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -799,7 +843,7 @@
     <col min="7" max="7" width="11.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18" style="6" customWidth="1"/>
     <col min="12" max="12" width="15.140625" style="6" customWidth="1"/>
     <col min="13" max="13" width="82.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="44.7109375" style="8" customWidth="1"/>
@@ -935,413 +979,413 @@
       <c r="M9" s="16"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="29">
-        <v>10</v>
-      </c>
-      <c r="E10" s="30">
+      <c r="C10" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="28">
+        <v>10</v>
+      </c>
+      <c r="E10" s="29">
         <v>0.85</v>
       </c>
-      <c r="F10" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="32">
-        <v>3</v>
-      </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33">
+      <c r="F10" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="31">
+        <v>3</v>
+      </c>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32">
         <v>0.7702</v>
       </c>
-      <c r="L10" s="28"/>
-      <c r="M10" s="36" t="s">
+      <c r="L10" s="27"/>
+      <c r="M10" s="35" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="29">
-        <v>10</v>
-      </c>
-      <c r="E11" s="30">
+      <c r="C11" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="28">
+        <v>10</v>
+      </c>
+      <c r="E11" s="29">
         <v>0.85</v>
       </c>
-      <c r="F11" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="32">
-        <v>5</v>
-      </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33">
+      <c r="F11" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="31">
+        <v>5</v>
+      </c>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32">
         <v>0.77029999999999998</v>
       </c>
-      <c r="L11" s="33"/>
-      <c r="M11" s="36" t="s">
+      <c r="L11" s="32"/>
+      <c r="M11" s="35" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="29">
-        <v>10</v>
-      </c>
-      <c r="E12" s="30">
+      <c r="C12" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="28">
+        <v>10</v>
+      </c>
+      <c r="E12" s="29">
         <v>0.75</v>
       </c>
-      <c r="F12" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="32">
-        <v>5</v>
-      </c>
-      <c r="J12" s="32"/>
-      <c r="K12" s="34">
+      <c r="F12" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="31">
+        <v>5</v>
+      </c>
+      <c r="J12" s="31"/>
+      <c r="K12" s="33">
         <v>0.78710000000000002</v>
       </c>
-      <c r="L12" s="34"/>
-      <c r="M12" s="36" t="s">
+      <c r="L12" s="33"/>
+      <c r="M12" s="35" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="28" t="s">
+      <c r="A13" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="29">
-        <v>10</v>
-      </c>
-      <c r="E13" s="30">
+      <c r="C13" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="28">
+        <v>10</v>
+      </c>
+      <c r="E13" s="29">
         <v>0.75</v>
       </c>
-      <c r="F13" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="31" t="s">
+      <c r="F13" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="32">
-        <v>5</v>
-      </c>
-      <c r="J13" s="32"/>
-      <c r="K13" s="35">
+      <c r="I13" s="31">
+        <v>5</v>
+      </c>
+      <c r="J13" s="31"/>
+      <c r="K13" s="34">
         <v>0.78220000000000001</v>
       </c>
-      <c r="L13" s="35"/>
-      <c r="M13" s="36" t="s">
+      <c r="L13" s="34"/>
+      <c r="M13" s="35" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="29">
-        <v>10</v>
-      </c>
-      <c r="E14" s="30">
+      <c r="D14" s="28">
+        <v>10</v>
+      </c>
+      <c r="E14" s="29">
         <v>0.5</v>
       </c>
-      <c r="F14" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="32">
-        <v>5</v>
-      </c>
-      <c r="J14" s="33">
+      <c r="F14" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="31">
+        <v>5</v>
+      </c>
+      <c r="J14" s="32">
         <v>0.86580000000000001</v>
       </c>
-      <c r="K14" s="33">
+      <c r="K14" s="32">
         <v>0.86785000000000001</v>
       </c>
-      <c r="L14" s="33" t="s">
+      <c r="L14" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="M14" s="37" t="s">
+      <c r="M14" s="36" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="28" t="s">
+      <c r="A15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="29">
-        <v>10</v>
-      </c>
-      <c r="E15" s="30">
+      <c r="C15" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="28">
+        <v>10</v>
+      </c>
+      <c r="E15" s="29">
         <v>0.75</v>
       </c>
-      <c r="F15" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="32">
-        <v>5</v>
-      </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33">
+      <c r="F15" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="31">
+        <v>5</v>
+      </c>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32">
         <v>0.78490000000000004</v>
       </c>
-      <c r="L15" s="33"/>
-      <c r="M15" s="37" t="s">
+      <c r="L15" s="32"/>
+      <c r="M15" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="28" t="s">
+      <c r="A16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="29">
-        <v>10</v>
-      </c>
-      <c r="E16" s="30">
+      <c r="C16" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="28">
+        <v>10</v>
+      </c>
+      <c r="E16" s="29">
         <v>0.72</v>
       </c>
-      <c r="F16" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="32">
-        <v>5</v>
-      </c>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33">
+      <c r="F16" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="31">
+        <v>5</v>
+      </c>
+      <c r="J16" s="31"/>
+      <c r="K16" s="32">
         <v>0.78290000000000004</v>
       </c>
-      <c r="L16" s="33"/>
-      <c r="M16" s="37" t="s">
+      <c r="L16" s="32"/>
+      <c r="M16" s="36" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="28" t="s">
+      <c r="A17" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="29">
-        <v>10</v>
-      </c>
-      <c r="E17" s="30">
+      <c r="C17" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="28">
+        <v>10</v>
+      </c>
+      <c r="E17" s="29">
         <v>0.82</v>
       </c>
-      <c r="F17" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="32">
-        <v>5</v>
-      </c>
-      <c r="J17" s="32"/>
-      <c r="K17" s="33">
+      <c r="F17" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="31">
+        <v>5</v>
+      </c>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32">
         <v>0.7772</v>
       </c>
-      <c r="L17" s="33"/>
-      <c r="M17" s="38" t="s">
+      <c r="L17" s="32"/>
+      <c r="M17" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="28" t="s">
+      <c r="A18" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="29">
-        <v>10</v>
-      </c>
-      <c r="E18" s="30">
+      <c r="C18" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="28">
+        <v>10</v>
+      </c>
+      <c r="E18" s="29">
         <v>0.75</v>
       </c>
-      <c r="F18" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="32">
-        <v>5</v>
-      </c>
-      <c r="J18" s="32"/>
-      <c r="K18" s="33">
+      <c r="F18" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="31">
+        <v>5</v>
+      </c>
+      <c r="J18" s="31"/>
+      <c r="K18" s="32">
         <v>0.78220000000000001</v>
       </c>
-      <c r="L18" s="33"/>
-      <c r="M18" s="36" t="s">
+      <c r="L18" s="32"/>
+      <c r="M18" s="35" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="28" t="s">
+      <c r="A19" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="29">
-        <v>10</v>
-      </c>
-      <c r="E19" s="30">
+      <c r="C19" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="28">
+        <v>10</v>
+      </c>
+      <c r="E19" s="29">
         <v>0.75</v>
       </c>
-      <c r="F19" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="32">
-        <v>5</v>
-      </c>
-      <c r="J19" s="32"/>
-      <c r="K19" s="33">
+      <c r="F19" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="31">
+        <v>5</v>
+      </c>
+      <c r="J19" s="31"/>
+      <c r="K19" s="32">
         <v>0.78549999999999998</v>
       </c>
-      <c r="L19" s="33"/>
-      <c r="M19" s="36" t="s">
+      <c r="L19" s="32"/>
+      <c r="M19" s="35" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="29">
-        <v>10</v>
-      </c>
-      <c r="E20" s="30">
+      <c r="C20" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="28">
+        <v>10</v>
+      </c>
+      <c r="E20" s="29">
         <v>0.75</v>
       </c>
-      <c r="F20" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="32">
-        <v>5</v>
-      </c>
-      <c r="J20" s="32"/>
-      <c r="K20" s="33">
+      <c r="F20" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="31">
+        <v>5</v>
+      </c>
+      <c r="J20" s="31"/>
+      <c r="K20" s="32">
         <v>0.77476999999999996</v>
       </c>
-      <c r="L20" s="33"/>
-      <c r="M20" s="36" t="s">
+      <c r="L20" s="32"/>
+      <c r="M20" s="35" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1368,7 +1412,7 @@
       <c r="B23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="3">
@@ -1407,7 +1451,7 @@
       <c r="B24" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D24" s="3">
@@ -1445,7 +1489,7 @@
       <c r="B25" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D25" s="3">
@@ -1483,7 +1527,7 @@
       <c r="B26" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="3">
@@ -1521,7 +1565,7 @@
       <c r="B27" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D27" s="3">
@@ -1559,7 +1603,7 @@
       <c r="B28" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D28" s="3">
@@ -1587,7 +1631,7 @@
         <v>0.78739999999999999</v>
       </c>
       <c r="L28" s="19"/>
-      <c r="M28" s="39" t="s">
+      <c r="M28" s="38" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1605,7 +1649,7 @@
         <v>10</v>
       </c>
       <c r="E29" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>5</v>
@@ -1622,17 +1666,17 @@
       <c r="J29" s="6">
         <v>0.86594000000000004</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="24">
         <v>0.86790500000000004</v>
       </c>
-      <c r="L29" s="25" t="s">
+      <c r="L29" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="M29" s="39" t="s">
+      <c r="M29" s="38" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>7</v>
       </c>
@@ -1646,7 +1690,7 @@
         <v>10</v>
       </c>
       <c r="E30" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>5</v>
@@ -1663,13 +1707,13 @@
       <c r="J30" s="6">
         <v>0.86591300000000004</v>
       </c>
-      <c r="K30" s="25">
+      <c r="K30" s="24">
         <v>0.86795999999999995</v>
       </c>
-      <c r="L30" s="25" t="s">
+      <c r="L30" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M30" s="39" t="s">
+      <c r="M30" s="38" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1687,7 +1731,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>5</v>
@@ -1704,13 +1748,13 @@
       <c r="J31" s="6">
         <v>0.86590999999999996</v>
       </c>
-      <c r="K31" s="25">
+      <c r="K31" s="24">
         <v>0.86807000000000001</v>
       </c>
-      <c r="L31" s="25" t="s">
+      <c r="L31" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="M31" s="39" t="s">
+      <c r="M31" s="38" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1721,7 +1765,7 @@
       <c r="B32" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="3">
@@ -1745,13 +1789,13 @@
       <c r="J32" s="6">
         <v>0.86614999999999998</v>
       </c>
-      <c r="K32" s="25">
+      <c r="K32" s="24">
         <v>0.86812</v>
       </c>
-      <c r="L32" s="25" t="s">
+      <c r="L32" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="M32" s="39" t="s">
+      <c r="M32" s="38" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1762,7 +1806,7 @@
       <c r="B33" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D33" s="3">
@@ -1786,17 +1830,17 @@
       <c r="J33" s="6">
         <v>0.8659</v>
       </c>
-      <c r="K33" s="25">
+      <c r="K33" s="24">
         <v>0.86817</v>
       </c>
-      <c r="L33" s="25" t="s">
+      <c r="L33" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M33" s="39" t="s">
+      <c r="M33" s="38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>7</v>
       </c>
@@ -1810,7 +1854,7 @@
         <v>10</v>
       </c>
       <c r="E34" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>5</v>
@@ -1827,17 +1871,17 @@
       <c r="J34" s="6">
         <v>0.865873</v>
       </c>
-      <c r="K34" s="25">
+      <c r="K34" s="24">
         <v>0.86824199999999996</v>
       </c>
-      <c r="L34" s="25" t="s">
+      <c r="L34" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="M34" s="39" t="s">
+      <c r="M34" s="38" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>7</v>
       </c>
@@ -1851,7 +1895,7 @@
         <v>10</v>
       </c>
       <c r="E35" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>5</v>
@@ -1868,13 +1912,13 @@
       <c r="J35" s="6">
         <v>0.86592000000000002</v>
       </c>
-      <c r="K35" s="25">
+      <c r="K35" s="24">
         <v>0.86827900000000002</v>
       </c>
-      <c r="L35" s="25" t="s">
+      <c r="L35" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M35" s="39" t="s">
+      <c r="M35" s="38" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1906,16 +1950,16 @@
       <c r="I36" s="18">
         <v>5</v>
       </c>
-      <c r="J36" s="25">
+      <c r="J36" s="24">
         <v>0.86606000000000005</v>
       </c>
-      <c r="K36" s="25">
+      <c r="K36" s="24">
         <v>0.868286</v>
       </c>
-      <c r="L36" s="25" t="s">
+      <c r="L36" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M36" s="39" t="s">
+      <c r="M36" s="38" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1926,7 +1970,7 @@
       <c r="B37" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D37" s="3">
@@ -1947,16 +1991,16 @@
       <c r="I37" s="18">
         <v>5</v>
       </c>
-      <c r="J37" s="25">
+      <c r="J37" s="24">
         <v>0.86602999999999997</v>
       </c>
-      <c r="K37" s="25">
+      <c r="K37" s="24">
         <v>0.86830099999999999</v>
       </c>
-      <c r="L37" s="25" t="s">
+      <c r="L37" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M37" s="39" t="s">
+      <c r="M37" s="38" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1988,20 +2032,20 @@
       <c r="I38" s="18">
         <v>5</v>
       </c>
-      <c r="J38" s="25">
+      <c r="J38" s="24">
         <v>0.86614000000000002</v>
       </c>
-      <c r="K38" s="25">
+      <c r="K38" s="24">
         <v>0.86831000000000003</v>
       </c>
-      <c r="L38" s="25" t="s">
+      <c r="L38" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M38" s="39" t="s">
+      <c r="M38" s="38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +2059,7 @@
         <v>10</v>
       </c>
       <c r="E39" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>5</v>
@@ -2032,17 +2076,17 @@
       <c r="J39" s="6">
         <v>0.86601399999999995</v>
       </c>
-      <c r="K39" s="25">
+      <c r="K39" s="24">
         <v>0.86833899999999997</v>
       </c>
-      <c r="L39" s="25" t="s">
+      <c r="L39" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="M39" s="39" t="s">
+      <c r="M39" s="38" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>7</v>
       </c>
@@ -2056,7 +2100,7 @@
         <v>10</v>
       </c>
       <c r="E40" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>5</v>
@@ -2073,13 +2117,13 @@
       <c r="J40" s="6">
         <v>0.86606000000000005</v>
       </c>
-      <c r="K40" s="25">
+      <c r="K40" s="24">
         <v>0.86841699999999999</v>
       </c>
-      <c r="L40" s="25" t="s">
+      <c r="L40" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="M40" s="39" t="s">
+      <c r="M40" s="38" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2111,16 +2155,16 @@
       <c r="I41" s="18">
         <v>5</v>
       </c>
-      <c r="J41" s="25">
+      <c r="J41" s="24">
         <v>0.86621000000000004</v>
       </c>
-      <c r="K41" s="25">
+      <c r="K41" s="24">
         <v>0.86843999999999999</v>
       </c>
-      <c r="L41" s="25" t="s">
+      <c r="L41" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="M41" s="39" t="s">
+      <c r="M41" s="38" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2152,20 +2196,20 @@
       <c r="I42" s="18">
         <v>5</v>
       </c>
-      <c r="J42" s="25">
+      <c r="J42" s="24">
         <v>0.86626000000000003</v>
       </c>
-      <c r="K42" s="25">
+      <c r="K42" s="24">
         <v>0.86845000000000006</v>
       </c>
-      <c r="L42" s="25" t="s">
+      <c r="L42" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="M42" s="39" t="s">
+      <c r="M42" s="38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>7</v>
       </c>
@@ -2179,7 +2223,7 @@
         <v>10</v>
       </c>
       <c r="E43" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>5</v>
@@ -2196,13 +2240,13 @@
       <c r="J43" s="6">
         <v>0.86602599999999996</v>
       </c>
-      <c r="K43" s="25">
+      <c r="K43" s="24">
         <v>0.86849299999999996</v>
       </c>
-      <c r="L43" s="25" t="s">
+      <c r="L43" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="M43" s="39" t="s">
+      <c r="M43" s="38" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2234,16 +2278,16 @@
       <c r="I44" s="18">
         <v>5</v>
       </c>
-      <c r="J44" s="25">
+      <c r="J44" s="24">
         <v>0.86626999999999998</v>
       </c>
-      <c r="K44" s="25">
+      <c r="K44" s="24">
         <v>0.86851</v>
       </c>
-      <c r="L44" s="25" t="s">
+      <c r="L44" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="M44" s="39" t="s">
+      <c r="M44" s="38" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2275,16 +2319,16 @@
       <c r="I45" s="18">
         <v>5</v>
       </c>
-      <c r="J45" s="25">
+      <c r="J45" s="24">
         <v>0.86641000000000001</v>
       </c>
-      <c r="K45" s="25">
+      <c r="K45" s="24">
         <v>0.86855000000000004</v>
       </c>
-      <c r="L45" s="25" t="s">
+      <c r="L45" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="M45" s="39" t="s">
+      <c r="M45" s="38" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2316,16 +2360,16 @@
       <c r="I46" s="18">
         <v>5</v>
       </c>
-      <c r="J46" s="25">
+      <c r="J46" s="24">
         <v>0.86641999999999997</v>
       </c>
-      <c r="K46" s="25">
+      <c r="K46" s="24">
         <v>0.86856999999999995</v>
       </c>
-      <c r="L46" s="25" t="s">
+      <c r="L46" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="M46" s="39" t="s">
+      <c r="M46" s="38" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2357,16 +2401,16 @@
       <c r="I47" s="18">
         <v>5</v>
       </c>
-      <c r="J47" s="25">
+      <c r="J47" s="24">
         <v>0.86643000000000003</v>
       </c>
-      <c r="K47" s="25">
+      <c r="K47" s="24">
         <v>0.86858000000000002</v>
       </c>
-      <c r="L47" s="25" t="s">
+      <c r="L47" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="M47" s="39" t="s">
+      <c r="M47" s="38" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2398,30 +2442,223 @@
       <c r="I48" s="18">
         <v>5</v>
       </c>
-      <c r="J48" s="26">
+      <c r="J48" s="25">
         <v>0.86643000000000003</v>
       </c>
-      <c r="K48" s="26">
+      <c r="K48" s="25">
         <v>0.86858999999999997</v>
       </c>
-      <c r="L48" s="26" t="s">
+      <c r="L48" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="M48" s="39" t="s">
+      <c r="M48" s="38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M49" s="39"/>
-    </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M50" s="39"/>
-    </row>
-    <row r="51" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M51" s="24"/>
-    </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M52" s="24"/>
+    <row r="49" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" s="3">
+        <v>10</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I49" s="18">
+        <v>5</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K49" s="6">
+        <v>0.86736500000000005</v>
+      </c>
+      <c r="L49" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="M49" s="38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="3">
+        <v>10</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I50" s="18">
+        <v>5</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K50" s="6">
+        <v>0.86737699999999995</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M50" s="38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="3">
+        <v>10</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I51" s="18">
+        <v>5</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K51" s="6">
+        <v>0.86531800000000003</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M51" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="3">
+        <v>10</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I52" s="18">
+        <v>5</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K52" s="6">
+        <v>0.867367</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M52" s="38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="3">
+        <v>10</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I53" s="18">
+        <v>5</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K53" s="6">
+        <v>0.86504700000000001</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M53" s="38" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A23:M48">

</xml_diff>

<commit_message>
updated Algo results sheet
</commit_message>
<xml_diff>
--- a/Consumer Debt Kaggle - Algo-Results.xlsx
+++ b/Consumer Debt Kaggle - Algo-Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="102">
   <si>
     <t>Algorithm</t>
   </si>
@@ -327,6 +327,24 @@
   <si>
     <t>GBM - max_features = 0.2, XGB - Best combination from Hyperopt
 Used cs-training-outlier-debt-f09 &amp; cs-test-outlier-debt-f09  files</t>
+  </si>
+  <si>
+    <t>GBM, RF</t>
+  </si>
+  <si>
+    <t>GBM - BayesOpt + Manual,
+RF - BayesOpt</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>0.866418</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBM: n_estimators=197, max_depth=5,  min_samples_split=319,  min_samples_leaf=89,  max_features=0.2, random_state=seed
+RF: n_estimators=161, criterion='gini', min_samples_split=223, min_samples_leaf=9, max_features=1, max_depth=14, random_state=seed
+</t>
   </si>
 </sst>
 </file>
@@ -825,11 +843,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M55" sqref="M55"/>
+      <pane ySplit="3" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -843,7 +861,7 @@
     <col min="7" max="7" width="11.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" style="6" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" style="6" customWidth="1"/>
     <col min="12" max="12" width="15.140625" style="6" customWidth="1"/>
     <col min="13" max="13" width="82.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="44.7109375" style="8" customWidth="1"/>
@@ -2660,6 +2678,47 @@
         <v>96</v>
       </c>
     </row>
+    <row r="55" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="3">
+        <v>10</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I55" s="18">
+        <v>5</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K55" s="6">
+        <v>0.86899800000000005</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M55" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A23:M48">
     <sortCondition ref="K23:K48"/>

</xml_diff>